<commit_message>
Add the pyrene lab and update some spreadsheets
</commit_message>
<xml_diff>
--- a/Diatomics.xlsx
+++ b/Diatomics.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20395"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matthewrowley1\Desktop\3625\Computation_Lab\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matthewrowley1\Desktop\3625\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{40DA98C3-232A-4B0C-88D6-2CC564F825D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81EAECB4-42FC-473E-84B1-62B1B17DA102}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="H2Scan" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3714,11 +3714,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="H96" sqref="H96:K101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>